<commit_message>
Visual Update on Class Code & File Update
</commit_message>
<xml_diff>
--- a/Excel/Bulanan/Excel/List Tugas Bulanan Ke-2 (30 Juli 2021 - 27 September 2021).xlsx
+++ b/Excel/Bulanan/Excel/List Tugas Bulanan Ke-2 (30 Juli 2021 - 27 September 2021).xlsx
@@ -1284,7 +1284,11 @@
         </is>
       </c>
       <c r="C17" s="28" t="inlineStr"/>
-      <c r="D17" s="33" t="inlineStr"/>
+      <c r="D17" s="31" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="E17" s="30" t="inlineStr">
         <is>
           <t>ü</t>
@@ -1904,8 +1908,16 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="G34" s="28" t="inlineStr"/>
-      <c r="H34" s="32" t="inlineStr"/>
+      <c r="G34" s="30" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
+      <c r="H34" s="34" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="I34" s="37" t="inlineStr">
         <is>
           <t>ü</t>

</xml_diff>

<commit_message>
Download Feature & File Update
</commit_message>
<xml_diff>
--- a/Excel/Bulanan/Excel/List Tugas Bulanan Ke-2 (30 Juli 2021 - 27 September 2021).xlsx
+++ b/Excel/Bulanan/Excel/List Tugas Bulanan Ke-2 (30 Juli 2021 - 27 September 2021).xlsx
@@ -1134,7 +1134,11 @@
       <c r="G11" s="28" t="inlineStr"/>
       <c r="H11" s="32" t="inlineStr"/>
       <c r="I11" s="29" t="inlineStr"/>
-      <c r="J11" s="32" t="inlineStr"/>
+      <c r="J11" s="34" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="12" ht="15.6" customHeight="1">
       <c r="A12" s="20" t="n">
@@ -1214,7 +1218,11 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="J13" s="32" t="inlineStr"/>
+      <c r="J13" s="34" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="14" ht="15.6" customHeight="1">
       <c r="A14" s="20" t="n">
@@ -1436,7 +1444,11 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="J18" s="32" t="inlineStr"/>
+      <c r="J18" s="34" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="19" ht="15.6" customHeight="1">
       <c r="A19" s="20" t="n">
@@ -1463,7 +1475,11 @@
         </is>
       </c>
       <c r="F19" s="33" t="inlineStr"/>
-      <c r="G19" s="28" t="inlineStr"/>
+      <c r="G19" s="30" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="H19" s="32" t="inlineStr"/>
       <c r="I19" s="37" t="inlineStr">
         <is>
@@ -1644,9 +1660,17 @@
       </c>
       <c r="F23" s="33" t="inlineStr"/>
       <c r="G23" s="28" t="inlineStr"/>
-      <c r="H23" s="32" t="inlineStr"/>
+      <c r="H23" s="34" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="I23" s="29" t="inlineStr"/>
-      <c r="J23" s="32" t="inlineStr"/>
+      <c r="J23" s="34" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="24" ht="15.6" customHeight="1">
       <c r="A24" s="20" t="n">
@@ -1940,7 +1964,11 @@
       <c r="G30" s="28" t="inlineStr"/>
       <c r="H30" s="32" t="inlineStr"/>
       <c r="I30" s="29" t="inlineStr"/>
-      <c r="J30" s="32" t="inlineStr"/>
+      <c r="J30" s="34" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="31" ht="15.6" customHeight="1">
       <c r="A31" s="20" t="n">

</xml_diff>

<commit_message>
Higher Excel Logo Resolution & File Update
</commit_message>
<xml_diff>
--- a/Excel/Bulanan/Excel/List Tugas Bulanan Ke-2 (30 Juli 2021 - 27 September 2021).xlsx
+++ b/Excel/Bulanan/Excel/List Tugas Bulanan Ke-2 (30 Juli 2021 - 27 September 2021).xlsx
@@ -1084,9 +1084,21 @@
         </is>
       </c>
       <c r="C9" s="28" t="inlineStr"/>
-      <c r="D9" s="33" t="inlineStr"/>
-      <c r="E9" s="28" t="inlineStr"/>
-      <c r="F9" s="33" t="inlineStr"/>
+      <c r="D9" s="31" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
+      <c r="E9" s="30" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
+      <c r="F9" s="31" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="G9" s="28" t="inlineStr"/>
       <c r="H9" s="32" t="inlineStr"/>
       <c r="I9" s="37" t="inlineStr">
@@ -1705,7 +1717,11 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="I23" s="29" t="inlineStr"/>
+      <c r="I23" s="37" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="J23" s="34" t="inlineStr">
         <is>
           <t>ü</t>
@@ -1784,7 +1800,11 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="H25" s="32" t="inlineStr"/>
+      <c r="H25" s="34" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="I25" s="37" t="inlineStr">
         <is>
           <t>ü</t>
@@ -1921,7 +1941,11 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="G28" s="28" t="inlineStr"/>
+      <c r="G28" s="30" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="H28" s="34" t="inlineStr">
         <is>
           <t>ü</t>

</xml_diff>

<commit_message>
Week 9 In Month 2 Text Correction & File Update
</commit_message>
<xml_diff>
--- a/Excel/Bulanan/Excel/List Tugas Bulanan Ke-2 (30 Juli 2021 - 27 September 2021).xlsx
+++ b/Excel/Bulanan/Excel/List Tugas Bulanan Ke-2 (30 Juli 2021 - 27 September 2021).xlsx
@@ -838,7 +838,7 @@
       <c r="O1" s="31" t="n"/>
       <c r="P1" s="51" t="inlineStr">
         <is>
-          <t>Minggu Ke-5</t>
+          <t>Minggu Ke-9</t>
         </is>
       </c>
       <c r="Q1" s="51" t="n"/>
@@ -1132,13 +1132,21 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="L5" s="44" t="inlineStr"/>
+      <c r="L5" s="47" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="M5" s="45" t="inlineStr">
         <is>
           <t>ü</t>
         </is>
       </c>
-      <c r="N5" s="44" t="inlineStr"/>
+      <c r="N5" s="47" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="O5" s="45" t="inlineStr">
         <is>
           <t>ü</t>
@@ -2099,13 +2107,21 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="L20" s="44" t="inlineStr"/>
+      <c r="L20" s="47" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="M20" s="45" t="inlineStr">
         <is>
           <t>ü</t>
         </is>
       </c>
-      <c r="N20" s="44" t="inlineStr"/>
+      <c r="N20" s="47" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="O20" s="45" t="inlineStr">
         <is>
           <t>ü</t>

</xml_diff>

<commit_message>
Angle Up To Down Animation & Other Page Some Banner Not Showing Bug Fixed
</commit_message>
<xml_diff>
--- a/Excel/Bulanan/Excel/List Tugas Bulanan Ke-2 (30 Juli 2021 - 27 September 2021).xlsx
+++ b/Excel/Bulanan/Excel/List Tugas Bulanan Ke-2 (30 Juli 2021 - 27 September 2021).xlsx
@@ -1203,7 +1203,11 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="T5" s="54" t="inlineStr"/>
+      <c r="T5" s="55" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="15.6" customHeight="1">
       <c r="A6" s="27" t="n">
@@ -3005,7 +3009,11 @@
       </c>
       <c r="P29" s="54" t="inlineStr"/>
       <c r="Q29" s="53" t="inlineStr"/>
-      <c r="R29" s="54" t="inlineStr"/>
+      <c r="R29" s="55" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="S29" s="53" t="inlineStr">
         <is>
           <t>NON-MUS</t>

</xml_diff>

<commit_message>
Code On Main Container Optimize
</commit_message>
<xml_diff>
--- a/Excel/Bulanan/Excel/List Tugas Bulanan Ke-2 (30 Juli 2021 - 27 September 2021).xlsx
+++ b/Excel/Bulanan/Excel/List Tugas Bulanan Ke-2 (30 Juli 2021 - 27 September 2021).xlsx
@@ -2430,8 +2430,16 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="T20" s="55" t="inlineStr"/>
-      <c r="U20" s="48" t="inlineStr"/>
+      <c r="T20" s="57" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
+      <c r="U20" s="56" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="21" ht="15.6" customHeight="1">
       <c r="A21" s="33" t="n">
@@ -2819,7 +2827,11 @@
           <t>ü</t>
         </is>
       </c>
-      <c r="T25" s="55" t="inlineStr"/>
+      <c r="T25" s="57" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="U25" s="56" t="inlineStr">
         <is>
           <t>ü</t>
@@ -3084,7 +3096,11 @@
       </c>
       <c r="P28" s="55" t="inlineStr"/>
       <c r="Q28" s="48" t="inlineStr"/>
-      <c r="R28" s="55" t="inlineStr"/>
+      <c r="R28" s="57" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="S28" s="56" t="inlineStr">
         <is>
           <t>ü</t>
@@ -3642,7 +3658,11 @@
         </is>
       </c>
       <c r="T35" s="55" t="inlineStr"/>
-      <c r="U35" s="48" t="inlineStr"/>
+      <c r="U35" s="56" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
     </row>
     <row r="36" ht="15.6" customHeight="1">
       <c r="A36" s="33" t="n">

</xml_diff>

<commit_message>
Content Text Justified In Changelog Page
</commit_message>
<xml_diff>
--- a/Excel/Bulanan/Excel/List Tugas Bulanan Ke-2 (30 Juli 2021 - 27 September 2021).xlsx
+++ b/Excel/Bulanan/Excel/List Tugas Bulanan Ke-2 (30 Juli 2021 - 27 September 2021).xlsx
@@ -3861,7 +3861,11 @@
       </c>
       <c r="P37" s="55" t="inlineStr"/>
       <c r="Q37" s="48" t="inlineStr"/>
-      <c r="R37" s="55" t="inlineStr"/>
+      <c r="R37" s="57" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="S37" s="56" t="inlineStr">
         <is>
           <t>ü</t>

</xml_diff>

<commit_message>
Bigger Font Size For Lower Screen Resolution & Improved The Responsiveness Of The Web
</commit_message>
<xml_diff>
--- a/Excel/Bulanan/Excel/List Tugas Bulanan Ke-2 (30 Juli 2021 - 27 September 2021).xlsx
+++ b/Excel/Bulanan/Excel/List Tugas Bulanan Ke-2 (30 Juli 2021 - 27 September 2021).xlsx
@@ -1253,7 +1253,11 @@
       </c>
       <c r="P5" s="55" t="inlineStr"/>
       <c r="Q5" s="48" t="inlineStr"/>
-      <c r="R5" s="55" t="inlineStr"/>
+      <c r="R5" s="57" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="S5" s="56" t="inlineStr">
         <is>
           <t>ü</t>
@@ -1508,7 +1512,11 @@
       </c>
       <c r="P8" s="55" t="inlineStr"/>
       <c r="Q8" s="48" t="inlineStr"/>
-      <c r="R8" s="55" t="inlineStr"/>
+      <c r="R8" s="57" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="S8" s="56" t="inlineStr">
         <is>
           <t>ü</t>
@@ -2436,7 +2444,11 @@
       </c>
       <c r="P20" s="55" t="inlineStr"/>
       <c r="Q20" s="48" t="inlineStr"/>
-      <c r="R20" s="55" t="inlineStr"/>
+      <c r="R20" s="57" t="inlineStr">
+        <is>
+          <t>ü</t>
+        </is>
+      </c>
       <c r="S20" s="56" t="inlineStr">
         <is>
           <t>ü</t>

</xml_diff>